<commit_message>
feat: echo; Added Sphinx support
</commit_message>
<xml_diff>
--- a/example_output.xlsx
+++ b/example_output.xlsx
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K2" t="n">
         <v>4</v>
@@ -565,7 +565,7 @@
         <v>2</v>
       </c>
       <c r="N2" t="n">
-        <v>3</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="O2" t="n">
         <v>4</v>
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H3" t="n">
         <v>4</v>
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K3" t="n">
         <v>4</v>
@@ -623,10 +623,10 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N3" t="n">
-        <v>7</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="O3" t="n">
         <v>4</v>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H4" t="n">
         <v>4</v>
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K4" t="n">
         <v>4</v>
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N4" t="n">
-        <v>7.333333333333333</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="O4" t="n">
         <v>4</v>
@@ -723,7 +723,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H5" t="n">
         <v>4</v>
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K5" t="n">
         <v>4</v>
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N5" t="n">
-        <v>4</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="O5" t="n">
         <v>4</v>
@@ -806,10 +806,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N6" t="n">
-        <v>8.666666666666666</v>
+        <v>7</v>
       </c>
       <c r="O6" t="n">
         <v>4</v>
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
         <v>4</v>
@@ -856,7 +856,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>4</v>
@@ -867,10 +867,10 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N7" t="n">
-        <v>4.333333333333333</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="O7" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
unknown, archive after quitting phd
</commit_message>
<xml_diff>
--- a/example_output.xlsx
+++ b/example_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N2" t="n">
-        <v>5.666666666666667</v>
+        <v>8</v>
       </c>
       <c r="O2" t="n">
         <v>4</v>
@@ -601,32 +601,32 @@
         </is>
       </c>
       <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>E:\MatrixTest\cmd_example_program.py</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>10</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>E:\MatrixTest\cmd_example_program.py</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
         <v>5</v>
       </c>
-      <c r="H3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>5</v>
-      </c>
-      <c r="K3" t="n">
-        <v>4</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="M3" t="n">
-        <v>6</v>
-      </c>
       <c r="N3" t="n">
-        <v>5.333333333333333</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="O3" t="n">
         <v>4</v>
@@ -673,206 +673,23 @@
         </is>
       </c>
       <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>E:\MatrixTest\cmd_example_program.py</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
         <v>8</v>
-      </c>
-      <c r="K4" t="n">
-        <v>4</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>4</v>
       </c>
       <c r="N4" t="n">
         <v>5.666666666666667</v>
       </c>
       <c r="O4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>python E:\MatrixTest\cmd_example_program.py arg1_2 arg2_1 arg3_1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>arg1_2</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>arg2_1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>arg3_1</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>7</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>4</v>
-      </c>
-      <c r="K5" t="n">
-        <v>4</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>2</v>
-      </c>
-      <c r="N5" t="n">
-        <v>4.333333333333333</v>
-      </c>
-      <c r="O5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>python E:\MatrixTest\cmd_example_program.py arg1_2 arg2_2 arg3_1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>arg1_2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>arg2_2</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>arg3_1</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>9</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>7</v>
-      </c>
-      <c r="K6" t="n">
-        <v>4</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>5</v>
-      </c>
-      <c r="N6" t="n">
-        <v>7</v>
-      </c>
-      <c r="O6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>python E:\MatrixTest\cmd_example_program.py arg1_2 arg2_3 arg3_1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>arg1_2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>arg2_3</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>arg3_1</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>4</v>
-      </c>
-      <c r="H7" t="n">
-        <v>4</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>4</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>E:\MatrixTest\cmd_example_program.py</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" t="n">
-        <v>3.666666666666667</v>
-      </c>
-      <c r="O7" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>